<commit_message>
mostrar meteo en las horas de la carrera
</commit_message>
<xml_diff>
--- a/php/estadisticas_uo288066.xlsx
+++ b/php/estadisticas_uo288066.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sew2526\php\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A0AAA7-2346-41AC-9BE5-03D883788C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA05F479-33B3-48CA-B8A0-C73567CA8FBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13749" xr2:uid="{EDA6C373-C3B0-4FB2-93F3-0BDE48218607}"/>
+    <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13749" activeTab="5" xr2:uid="{EDA6C373-C3B0-4FB2-93F3-0BDE48218607}"/>
   </bookViews>
   <sheets>
     <sheet name="uo288066_db_resultados" sheetId="15" r:id="rId1"/>
@@ -26476,7 +26476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1D35FF4-9EB2-46CA-A15D-A2D625484CEA}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -27473,8 +27473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E26DE797-EEB2-4B58-B867-67BE01D99B3E}">
   <dimension ref="B1:R45"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:R45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -28953,8 +28953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{758C81DB-CDD8-4CF0-B995-68970B44831E}">
   <dimension ref="B1:AH35"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AA38" sqref="AA38"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>

</xml_diff>